<commit_message>
changed excel file and adding to a new branch
</commit_message>
<xml_diff>
--- a/GitPracticeFile.xlsx
+++ b/GitPracticeFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a01ac9f7c40eb0a/Desktop/git/Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77076FE1-509A-460B-9A3A-6A7D8FB18EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{77076FE1-509A-460B-9A3A-6A7D8FB18EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{640F8072-4153-4491-A769-F019A34AEA72}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-2604" windowWidth="30936" windowHeight="16776" xr2:uid="{8356CE65-87D2-4D29-81C9-543C3690CCA3}"/>
   </bookViews>
@@ -381,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75C04EA-7CE3-4E18-B74D-5BD34DEC8EFE}">
-  <dimension ref="B2:B5"/>
+  <dimension ref="B2:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,6 +409,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>